<commit_message>
More tests e asserting tests
</commit_message>
<xml_diff>
--- a/MeuPonto.Tests/meu_horario.xlsx
+++ b/MeuPonto.Tests/meu_horario.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,7 +822,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="D8" s="5">
-        <v>0.54861111111111105</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="E8" s="6">
         <v>0.59722222222222221</v>
@@ -831,30 +831,30 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="G8" s="5">
-        <v>0.78819444444444453</v>
+        <v>0.79375000000000007</v>
       </c>
       <c r="H8" s="5">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="I8" s="8">
         <f>IF(OR(D8="",E8=""),"",E8-D8)</f>
-        <v>4.861111111111116E-2</v>
+        <v>6.3888888888888884E-2</v>
       </c>
       <c r="J8" s="9">
         <f>IF(OR(F8="",G8=""),"",G8-F8)</f>
-        <v>1.736111111111116E-2</v>
+        <v>2.2916666666666696E-2</v>
       </c>
       <c r="K8" s="9">
         <f>IF(C8="","",(C8+'c'!$A$1)+IF(I8="",0,I8)+IF(J8="",0,J8))</f>
-        <v>0.53125000000000011</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="L8" s="18">
         <f>IF(H8="","",IF(C8&lt;H8,H8-C8,(1-C8)+H8)-IF(I8="",0,I8)-IF(J8="",0,J8))</f>
-        <v>0.85416666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M8" s="18">
         <f>IF(H8="","",IF(L8-'c'!$A$1&gt;0,L8-'c'!$A$1,""))</f>
-        <v>0.52083333333333326</v>
+        <v>0.5</v>
       </c>
       <c r="N8" s="18" t="str">
         <f>IF(H8="","",IF(L8-'c'!$A$1&lt;0,'c'!$A$1-L8,""))</f>
@@ -1851,11 +1851,11 @@
       <c r="K33" s="12"/>
       <c r="L33" s="16">
         <f>SUM(L2:L32)</f>
-        <v>2.1944444444444442</v>
+        <v>2.1736111111111107</v>
       </c>
       <c r="M33" s="16">
         <f>SUM(M2:M32)</f>
-        <v>0.6875</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="N33" s="16">
         <f>SUM(N2:N32)</f>
@@ -1864,7 +1864,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17">
         <f>M33-N33</f>
-        <v>0.52777777777777768</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="34" spans="1:20">

</xml_diff>

<commit_message>
Periodo class and more tests
</commit_message>
<xml_diff>
--- a/MeuPonto.Tests/meu_horario.xlsx
+++ b/MeuPonto.Tests/meu_horario.xlsx
@@ -495,10 +495,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="R9" sqref="R9:W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1837,7 +1837,7 @@
       <c r="O32" s="10"/>
       <c r="P32"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:16">
       <c r="A33" s="11"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1867,37 +1867,17 @@
         <v>0.50694444444444442</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="4"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="9"/>
-      <c r="P34" s="9"/>
-    </row>
-    <row r="36" spans="1:20">
-      <c r="K36" s="9"/>
-    </row>
-    <row r="37" spans="1:20">
-      <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="1:20">
-      <c r="K38" s="9"/>
-    </row>
-    <row r="39" spans="1:20">
-      <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="1:20">
-      <c r="T40" s="9"/>
-    </row>
-    <row r="41" spans="1:20">
-      <c r="G41" s="9"/>
-      <c r="T41" s="9"/>
-    </row>
-    <row r="42" spans="1:20">
-      <c r="T42" s="14"/>
-    </row>
-    <row r="43" spans="1:20">
-      <c r="T43" s="14"/>
+    <row r="40" spans="1:16">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="14"/>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>